<commit_message>
delete auth_type;fix datatable selectAll bug;
</commit_message>
<xml_diff>
--- a/upload/资产导入模板.xlsx
+++ b/upload/资产导入模板.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="62">
   <si>
     <t>服务器类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -77,10 +77,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>认证方式</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>用户密码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -173,6 +169,80 @@
   <si>
     <t>10.1.19.101</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JR002</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10.1.19.11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JR003</t>
+  </si>
+  <si>
+    <t>JR004</t>
+  </si>
+  <si>
+    <t>JR005</t>
+  </si>
+  <si>
+    <t>JR006</t>
+  </si>
+  <si>
+    <t>JR007</t>
+  </si>
+  <si>
+    <t>JR008</t>
+  </si>
+  <si>
+    <t>JR009</t>
+  </si>
+  <si>
+    <t>JR010</t>
+  </si>
+  <si>
+    <t>JR011</t>
+  </si>
+  <si>
+    <t>JR012</t>
+  </si>
+  <si>
+    <t>JR013</t>
+  </si>
+  <si>
+    <t>10.1.19.12</t>
+  </si>
+  <si>
+    <t>10.1.19.13</t>
+  </si>
+  <si>
+    <t>10.1.19.14</t>
+  </si>
+  <si>
+    <t>10.1.19.15</t>
+  </si>
+  <si>
+    <t>10.1.19.16</t>
+  </si>
+  <si>
+    <t>10.1.19.17</t>
+  </si>
+  <si>
+    <t>10.1.19.18</t>
+  </si>
+  <si>
+    <t>10.1.19.19</t>
+  </si>
+  <si>
+    <t>10.1.19.20</t>
+  </si>
+  <si>
+    <t>10.1.19.21</t>
+  </si>
+  <si>
+    <t>10.1.19.22</t>
   </si>
 </sst>
 </file>
@@ -537,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S4"/>
+  <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -551,13 +621,13 @@
     <col min="12" max="12" width="11.125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.25" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9" style="4"/>
-    <col min="18" max="18" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="9" style="4"/>
+    <col min="17" max="17" width="8.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -601,25 +671,22 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.15">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -628,7 +695,7 @@
         <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2">
         <v>2</v>
@@ -652,30 +719,27 @@
         <v>0</v>
       </c>
       <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="R2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J3" s="2">
         <v>39668</v>
@@ -686,31 +750,28 @@
       <c r="N3">
         <v>1</v>
       </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>35</v>
+      <c r="P3" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q3">
+        <v>22</v>
       </c>
       <c r="R3">
-        <v>22</v>
-      </c>
-      <c r="S3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="2">
         <v>39668</v>
@@ -721,22 +782,583 @@
       <c r="N4">
         <v>1</v>
       </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>35</v>
+      <c r="P4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4">
+        <v>22</v>
       </c>
       <c r="R4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K5" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L5">
+        <v>800</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q5">
         <v>22</v>
       </c>
-      <c r="S4">
-        <v>1</v>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K6" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L6">
+        <v>800</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6" t="s">
+        <v>23</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K7" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L7">
+        <v>800</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7" t="s">
+        <v>23</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K8" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L8">
+        <v>800</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>23</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q8">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K9" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L9">
+        <v>800</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9" t="s">
+        <v>23</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K10" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L10">
+        <v>800</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10" t="s">
+        <v>23</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K11" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L11">
+        <v>800</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>23</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>57</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K12" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L12">
+        <v>800</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12" t="s">
+        <v>23</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q12">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K13" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L13">
+        <v>800</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13" t="s">
+        <v>23</v>
+      </c>
+      <c r="P13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>59</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K14" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L14">
+        <v>800</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q14">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>60</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K15" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L15">
+        <v>800</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15" t="s">
+        <v>23</v>
+      </c>
+      <c r="P15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q15">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>61</v>
+      </c>
+      <c r="G16">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16" s="2">
+        <v>39668</v>
+      </c>
+      <c r="K16" s="2">
+        <v>43320</v>
+      </c>
+      <c r="L16">
+        <v>800</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16" t="s">
+        <v>23</v>
+      </c>
+      <c r="P16" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q16">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations xWindow="226" yWindow="274" count="15">
+  <dataValidations xWindow="226" yWindow="274" count="14">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="0 表示物理机_x000a_1 表示虚拟机_x000a_2 表示云主机" sqref="N2:N1048576">
       <formula1>"0,1,2"</formula1>
     </dataValidation>
@@ -744,7 +1366,7 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="输入整数，请确保输入的数值与数据库中对应供应商的ID一致" sqref="D2:D1048576">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 R1:S1 L1 G1:I1"/>
+    <dataValidation operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1 Q1:R1 L1 G1:I1"/>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="0 代表已上线_x000a_1 代表已下线_x000a_2 代表故障中_x000a_3 代表未使用" sqref="E2:E1048576">
       <formula1>"0,1,2,3"</formula1>
     </dataValidation>
@@ -758,13 +1380,10 @@
     <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2:L1048576">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="0 表示密钥认证_x000a_1 表示密码认证" sqref="P2:P1048576">
-      <formula1>"0,1"</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2:R1048576">
-      <formula1>1</formula1>
-    </dataValidation>
-    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="虚拟机专用字段，填入整数，确认所填数据与数据库中宿主机的ID一致" sqref="S2:S1048576">
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2:Q1048576">
+      <formula1>1</formula1>
+    </dataValidation>
+    <dataValidation type="whole" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="虚拟机专用字段，填入整数，确认所填数据与数据库中宿主机的ID一致" sqref="R2:R1048576">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="必填项，格式_x000a_1970-01-01" sqref="J2:K1048576">
@@ -802,7 +1421,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -841,18 +1460,18 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
         <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>28</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -861,7 +1480,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2">
         <v>1</v>
@@ -945,7 +1564,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -984,7 +1603,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
@@ -1051,7 +1670,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1090,7 +1709,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
@@ -1157,7 +1776,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1196,7 +1815,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">
@@ -1263,7 +1882,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -1302,7 +1921,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.15">

</xml_diff>